<commit_message>
Project Tutorial 7 - Introduction to Table Properties is saved. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Tutorial 7 - Introduction to Table Properties/Tutorial7 - Intro to Table Properties.xlsx
+++ b/DESIGN/rules/Tutorial 7 - Introduction to Table Properties/Tutorial7 - Intro to Table Properties.xlsx
@@ -171,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="151">
   <si>
     <t>Amount</t>
   </si>
@@ -1209,6 +1209,9 @@
       </rPr>
       <t xml:space="preserve"> (Car car, int numberOfCars, Address billingAddress)</t>
     </r>
+  </si>
+  <si>
+    <t>= CarPrice (car, billingAddress)+100</t>
   </si>
 </sst>
 </file>
@@ -1299,7 +1302,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="0" tint="-0.499984740745262"/>
+      <color theme="0" tint="-0.499984740745262" rgb="FFFFFF"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
       <charset val="204"/>
@@ -1410,7 +1413,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="0" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1422,7 +1425,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor theme="0" tint="-0.34998626667073579" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1434,7 +1437,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.14999847407452621" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1897,26 +1900,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+  <cellStyleXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" xfId="3">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6"/>
   </cellStyleXfs>
   <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1978,13 +1972,13 @@
     <xf numFmtId="3" fontId="5" fillId="4" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="24" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="24" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="25" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="25" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="26" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="26" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="5" fillId="4" borderId="31" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2014,10 +2008,10 @@
     <xf numFmtId="9" fontId="5" fillId="8" borderId="33" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="34" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="34" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="35" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="35" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2172,10 +2166,10 @@
     <xf numFmtId="3" fontId="5" fillId="4" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="21" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="21" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="22" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="22" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2193,7 +2187,7 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="23" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="23" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="5" fillId="4" borderId="30" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2227,23 +2221,14 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="16">
-    <cellStyle name="Heading 1 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+  <cellStyles count="7">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2 9" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 6" xfId="2" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Hyperlink 3" xfId="11" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="13" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal 2 9" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 3 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Normal 3 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Normal 3 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Normal 5" xfId="15" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Normal 6" xfId="2" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Normal 7" xfId="7" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="Normal 7 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="Normal 9" xfId="14" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="Обычный 2" xfId="6" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="Обычный 5" xfId="10" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Обычный 5" xfId="6" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2871,7 +2856,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.109375" style="3" collapsed="1"/>
+    <col min="1" max="16384" style="3" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:11" ht="22.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3193,12 +3178,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="1"/>
-    <col min="3" max="3" width="24.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="2" style="1" width="9.109375" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="1" width="24.109375" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="1" width="23.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="1" width="20.109375" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="1" width="13.88671875" collapsed="false"/>
+    <col min="7" max="16384" style="1" width="9.109375" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" ht="19.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3603,14 +3588,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.109375" style="1"/>
-    <col min="4" max="4" width="24.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.109375" style="1" customWidth="1"/>
-    <col min="8" max="12" width="18" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="3" style="1" width="9.109375" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="1" width="24.109375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="1" width="23.0" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="1" width="20.109375" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" style="1" width="21.109375" collapsed="false"/>
+    <col min="8" max="12" customWidth="true" style="1" width="18.0" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" style="1" width="11.109375" collapsed="false"/>
+    <col min="14" max="16384" style="1" width="9.109375" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:13" ht="19.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -5270,7 +5255,7 @@
         <v>99</v>
       </c>
       <c r="E81" s="103" t="s">
-        <v>96</v>
+        <v>150</v>
       </c>
       <c r="F81" s="103"/>
       <c r="G81" s="9"/>
@@ -6824,14 +6809,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="1"/>
-    <col min="3" max="3" width="24.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" style="1" customWidth="1"/>
-    <col min="7" max="8" width="21.109375" style="66" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" style="66" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="2" style="1" width="9.109375" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="1" width="24.109375" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="1" width="23.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="1" width="20.109375" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="1" width="21.109375" collapsed="false"/>
+    <col min="7" max="8" customWidth="true" style="66" width="21.109375" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" style="66" width="12.33203125" collapsed="false"/>
+    <col min="10" max="16384" style="1" width="9.109375" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:9" ht="19.2" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>